<commit_message>
pushing code for POM framework
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Opencart_testData.xlsx
+++ b/src/test/resources/testdata/Opencart_testData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanjayrastogi\Desktop\selenium data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C131FF8A-853E-49EC-8651-0D3E858F1331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA14D75-941C-41D8-BAB7-F8A394146388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A4FF639E-93FC-4BAA-BCB3-9960A92C0AD6}"/>
   </bookViews>
   <sheets>
     <sheet name="userRegistrationData" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,36 +59,18 @@
     <t>Somawar</t>
   </si>
   <si>
-    <t>chaitanya909@gmail.com</t>
-  </si>
-  <si>
-    <t>334534535</t>
-  </si>
-  <si>
-    <t>test@12121</t>
-  </si>
-  <si>
     <t>Madhurima</t>
   </si>
   <si>
     <t>lastname01</t>
   </si>
   <si>
-    <t>madhu9879879@gmail.com</t>
-  </si>
-  <si>
-    <t>test@12122</t>
-  </si>
-  <si>
     <t>Vaibhav</t>
   </si>
   <si>
     <t>lastname02</t>
   </si>
   <si>
-    <t>vaibhav0132@gmail.com</t>
-  </si>
-  <si>
     <t>test@12123</t>
   </si>
   <si>
@@ -97,19 +80,37 @@
     <t>Nikhil</t>
   </si>
   <si>
-    <t>4524525252</t>
-  </si>
-  <si>
-    <t>987937979</t>
-  </si>
-  <si>
-    <t>nikhilq325245@test.com</t>
-  </si>
-  <si>
-    <t>45252452452</t>
-  </si>
-  <si>
     <t>test@12124</t>
+  </si>
+  <si>
+    <t>334534112</t>
+  </si>
+  <si>
+    <t>test@322121</t>
+  </si>
+  <si>
+    <t>test@23412122</t>
+  </si>
+  <si>
+    <t>452452323233</t>
+  </si>
+  <si>
+    <t>9879378711</t>
+  </si>
+  <si>
+    <t>232387987</t>
+  </si>
+  <si>
+    <t>chaitanya234aa45@gmail.com</t>
+  </si>
+  <si>
+    <t>madhu898jkhkj179@gmail.com</t>
+  </si>
+  <si>
+    <t>vaibhav9utiut6549732@gmail.com</t>
+  </si>
+  <si>
+    <t>nikhilq3hjkytu7653445@test.com</t>
   </si>
 </sst>
 </file>
@@ -476,7 +477,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -510,64 +511,64 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -583,4 +584,16 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD79FEE3-F1B1-4ABD-997B-C01E9F8E8E76}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>